<commit_message>
Split images into folders
</commit_message>
<xml_diff>
--- a/bioassay_test/Ascochyta_rabiei_phenotyping_form_data.xlsx
+++ b/bioassay_test/Ascochyta_rabiei_phenotyping_form_data.xlsx
@@ -27554,6 +27554,8 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
     <TaxCatchAll xmlns="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
@@ -27568,8 +27570,9 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7a124c12a779a736f71215d7d4687bf">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2155876b7947a55992891bc9fceb70da" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8E840779CD5394DB6A0677C69D57CD3" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="759527f59e11d69b52594aee1565f7b2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1f3c66e0-7684-4412-85ae-938bcfc42664" xmlns:ns3="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfa3fb632320c027112c736c6f89e4dc" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="1f3c66e0-7684-4412-85ae-938bcfc42664"/>
     <xsd:import namespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29"/>
     <xsd:element name="properties">
@@ -27593,11 +27596,28 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="24" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="25" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1f3c66e0-7684-4412-85ae-938bcfc42664" elementFormDefault="qualified">
@@ -27668,6 +27688,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="26" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c30d4e8-d9db-43d6-83e2-c08e4749ca29" elementFormDefault="qualified">
@@ -27819,5 +27844,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A9DFA40-0AE7-44FD-8A5C-899EA7DDEE73}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F23F790A-8369-4C0A-92D5-89177304EABF}"/>
 </file>
</xml_diff>